<commit_message>
Atualizat templates , css
</commit_message>
<xml_diff>
--- a/data/output/relatorio_estoques.xlsx
+++ b/data/output/relatorio_estoques.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Preco Estimado</t>
+          <t>Preço Estimado</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -463,87 +463,87 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Higiene</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sabonete</t>
+          <t>arroz</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>15/09/2025 01:08</t>
+          <t>18/09/2025 01:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Laticínios</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CArne moida</t>
+          <t>bolacha choc mabel</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>25.00</t>
+          <t>7.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15/09/2025 01:06</t>
+          <t>18/09/2025 01:03</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Laticínios</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Coxinha da asa</t>
+          <t>papel toalha</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>50.00</t>
+          <t>7.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>15/09/2025 01:07</t>
+          <t>23/09/2025 02:19</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Reforma Casa</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Limpar armarios</t>
+          <t>guardanapo</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -551,37 +551,912 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.00</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>15/09/2025 02:35</t>
+          <t>23/09/2025 02:19</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reforma Casa</t>
+          <t>Alimentos</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>lampadas</t>
+          <t>feijão</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>8.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>15/09/2025 02:36</t>
+          <t>23/09/2025 02:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>leite Gaby</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>28.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>açúcar</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>18/09/2025 01:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>macarrão</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>6.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>18/09/2025 01:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>filtro café</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sal</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>12.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>suco grande</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>café</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>62.00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>24/09/2025 01:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Higiene</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>álcool</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Higiene</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sabão barra</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>9.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Higiene</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>bom bril</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Higiene</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>detergente pia</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Higiene</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>sabonete líquido</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Higiene</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>sabonete</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>24/09/2025 00:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Coxinha da asa</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>15/09/2025 01:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>leite</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>12.00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>carne moída</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>requeijão cremoso</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>13.00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>suco grante</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ovos cx</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>qeueijo zero</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Laticínios</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>suco pq Gaby</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>24/09/2025 01:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Manutenção casa</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Ralo do banheiro</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>23/09/2025 00:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Manutenção casa</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Limpar portas</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>23/09/2025 00:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Manutenção casa</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Limpar armários</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>23/09/2025 00:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Manutenção casa</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Comprar armário sala</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2000.00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>23/09/2025 00:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Manutenção casa</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>comprar escrevaninha</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>23/09/2025 00:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Manutenção casa</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Vender bicicleta</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>23/09/2025 00:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>pão de forma</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>6.00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>club social</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>6.00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>bolo wilk bold pr</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>bolacha choc zero</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>bisnaguinha</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>pão sal</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>23/09/2025 02:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ciabata</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Padaria</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mini óreon</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>5</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>23/09/2025 14:24</t>
         </is>
       </c>
     </row>

</xml_diff>